<commit_message>
user stories and sprint
</commit_message>
<xml_diff>
--- a/Documentation/Taskliste1.xlsx
+++ b/Documentation/Taskliste1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDant\GIT\ProjectWatch\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\cours\semestre 3\watch\ProjectWatch\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Tasknr.</t>
   </si>
@@ -84,12 +84,15 @@
   </si>
   <si>
     <t xml:space="preserve">Mise à jour des différents fichiers de documentation </t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -413,22 +416,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="87.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="32.19921875" customWidth="1"/>
+    <col min="5" max="5" width="32.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,74 +448,158 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>18</v>
+      </c>
+      <c r="C15">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>